<commit_message>
adding indo province level
</commit_message>
<xml_diff>
--- a/CovidBali/testingDash/plotly apps-dash-oil-and-gas/data/regencyCasesBali.xlsx
+++ b/CovidBali/testingDash/plotly apps-dash-oil-and-gas/data/regencyCasesBali.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansve\Coding\Projects-WebScraping\CovidBali\testingDash\plotly apps-dash-oil-and-gas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52D08E6-1368-4C92-A537-A80CA291DFA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F48FD2-BCDC-4839-8DC6-0E88C10C7578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="816" yWindow="1728" windowWidth="21612" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="504" yWindow="312" windowWidth="21612" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="81">
   <si>
     <t>Regency</t>
   </si>
@@ -477,6 +477,18 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Bali#Geography</t>
+  </si>
+  <si>
+    <t>mortality_rate</t>
+  </si>
+  <si>
+    <t>deaths_per_100k</t>
+  </si>
+  <si>
+    <t>cases7_per_100k</t>
+  </si>
+  <si>
+    <t>total_deaths</t>
   </si>
 </sst>
 </file>
@@ -661,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -695,13 +707,14 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1005,20 +1018,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.88671875" customWidth="1"/>
-    <col min="2" max="14" width="15" customWidth="1"/>
-    <col min="16" max="16" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="15.88671875" customWidth="1"/>
+    <col min="17" max="17" width="14.5546875" customWidth="1"/>
+    <col min="18" max="18" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1056,19 +1071,31 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>20201201</v>
       </c>
@@ -1105,22 +1132,33 @@
       <c r="L2" s="2">
         <v>645</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="2">
+        <v>5</v>
+      </c>
+      <c r="N2">
         <v>2.809559714635268</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>5</v>
       </c>
-      <c r="O2">
-        <f>L2/P2</f>
-        <v>2.3763645674832272</v>
-      </c>
       <c r="P2">
+        <f>L2/Q2*100</f>
+        <v>237.63645674832273</v>
+      </c>
+      <c r="Q2">
         <f>VLOOKUP(B2, references!$A$4:'references'!$G$12,7)</f>
         <v>271.423</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R2">
+        <f>M2/L2*100</f>
+        <v>0.77519379844961245</v>
+      </c>
+      <c r="S2">
+        <f>Q2/M2</f>
+        <v>54.284599999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>20201201</v>
       </c>
@@ -1157,22 +1195,29 @@
       <c r="L3" s="2">
         <v>1436</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="2">
+        <v>12</v>
+      </c>
+      <c r="N3">
         <v>3.157154439906281</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>9</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O34" si="0">L3/P3</f>
-        <v>3.2954448965354226</v>
-      </c>
       <c r="P3">
+        <f t="shared" ref="P3:P34" si="0">L3/Q3*100</f>
+        <v>329.54448965354226</v>
+      </c>
+      <c r="Q3">
         <f>VLOOKUP(B3, references!$A$4:'references'!$G$12,7)</f>
         <v>435.75299999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R3">
+        <f t="shared" ref="R3:R34" si="1">M3/L3*100</f>
+        <v>0.83565459610027859</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>20201201</v>
       </c>
@@ -1209,22 +1254,29 @@
       <c r="L4" s="2">
         <v>2467</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="2">
+        <v>25</v>
+      </c>
+      <c r="N4">
         <v>3.3921691494897361</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
         <v>1</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <f t="shared" si="0"/>
-        <v>4.0104170053385522</v>
-      </c>
-      <c r="P4">
+        <v>401.04170053385519</v>
+      </c>
+      <c r="Q4">
         <f>VLOOKUP(B4, references!$A$4:'references'!$G$12,7)</f>
         <v>615.14800000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R4">
+        <f t="shared" si="1"/>
+        <v>1.0133765707336846</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>20201201</v>
       </c>
@@ -1261,22 +1313,29 @@
       <c r="L5" s="2">
         <v>3916</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="16">
+        <v>88</v>
+      </c>
+      <c r="N5">
         <v>3.5928426831310998</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>8</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <f t="shared" si="0"/>
-        <v>22.304112819169234</v>
-      </c>
-      <c r="P5">
+        <v>2230.4112819169231</v>
+      </c>
+      <c r="Q5">
         <f>VLOOKUP(B5, references!$A$4:'references'!$G$12,7)</f>
         <v>175.57300000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R5">
+        <f t="shared" si="1"/>
+        <v>2.2471910112359552</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>20201201</v>
       </c>
@@ -1313,22 +1372,29 @@
       <c r="L6" s="2">
         <v>1962</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="16">
+        <v>5</v>
+      </c>
+      <c r="N6">
         <v>3.2926990030439298</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <v>4</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <f t="shared" si="0"/>
-        <v>3.9658075431195665</v>
-      </c>
-      <c r="P6">
+        <v>396.58075431195664</v>
+      </c>
+      <c r="Q6">
         <f>VLOOKUP(B6, references!$A$4:'references'!$G$12,7)</f>
         <v>494.72899999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R6">
+        <f t="shared" si="1"/>
+        <v>0.254841997961264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>20201201</v>
       </c>
@@ -1365,22 +1431,29 @@
       <c r="L7" s="2">
         <v>885</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="16">
+        <v>20</v>
+      </c>
+      <c r="N7">
         <v>2.946943270697826</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>2</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <f t="shared" si="0"/>
-        <v>3.9779929340057718</v>
-      </c>
-      <c r="P7">
+        <v>397.7992934005772</v>
+      </c>
+      <c r="Q7">
         <f>VLOOKUP(B7, references!$A$4:'references'!$G$12,7)</f>
         <v>222.47399999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R7">
+        <f t="shared" si="1"/>
+        <v>2.2598870056497176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>20201201</v>
       </c>
@@ -1417,22 +1490,29 @@
       <c r="L8" s="2">
         <v>944</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="16">
+        <v>25</v>
+      </c>
+      <c r="N8">
         <v>2.9749719942980688</v>
       </c>
-      <c r="N8" s="2">
+      <c r="O8" s="2">
         <v>7</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <f t="shared" si="0"/>
-        <v>5.3766809247435541</v>
-      </c>
-      <c r="P8">
+        <v>537.66809247435538</v>
+      </c>
+      <c r="Q8">
         <f>VLOOKUP(B8, references!$A$4:'references'!$G$12,7)</f>
         <v>175.57300000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R8">
+        <f t="shared" si="1"/>
+        <v>2.6483050847457625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>20201201</v>
       </c>
@@ -1469,22 +1549,29 @@
       <c r="L9" s="2">
         <v>1026</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="16">
+        <v>4</v>
+      </c>
+      <c r="N9">
         <v>3.011147360775797</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>6</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <f t="shared" si="0"/>
-        <v>2.5117078389275544</v>
-      </c>
-      <c r="P9">
+        <v>251.17078389275545</v>
+      </c>
+      <c r="Q9">
         <f>VLOOKUP(B9, references!$A$4:'references'!$G$12,7)</f>
         <v>408.48700000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>0.38986354775828458</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>20201201</v>
       </c>
@@ -1521,22 +1608,29 @@
       <c r="L10" s="2">
         <v>1206</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="16">
+        <v>1</v>
+      </c>
+      <c r="N10">
         <v>3.081347307804132</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>3</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <f t="shared" si="0"/>
-        <v>1.8671823351545844</v>
-      </c>
-      <c r="P10">
+        <v>186.71823351545845</v>
+      </c>
+      <c r="Q10">
         <f>VLOOKUP(B10, references!$A$4:'references'!$G$12,7)</f>
         <v>645.89300000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R10">
+        <f t="shared" si="1"/>
+        <v>8.2918739635157543E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>20201201</v>
       </c>
@@ -1573,22 +1667,29 @@
       <c r="L11" s="2">
         <v>49</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="16">
+        <v>2</v>
+      </c>
+      <c r="N11">
         <v>1.6901960800285141</v>
       </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
       <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="0"/>
-        <v>0.18053002140570254</v>
-      </c>
-      <c r="P11">
+        <v>18.053002140570253</v>
+      </c>
+      <c r="Q11">
         <f>VLOOKUP(B11, references!$A$4:'references'!$G$12,7)</f>
         <v>271.423</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>4.0816326530612246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>20201201</v>
       </c>
@@ -1625,22 +1726,29 @@
       <c r="L12" s="2">
         <v>32</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="16">
+        <v>10</v>
+      </c>
+      <c r="N12">
         <v>1.505149978319906</v>
       </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
       <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="0"/>
-        <v>7.3436097972934211E-2</v>
-      </c>
-      <c r="P12">
+        <v>7.3436097972934213</v>
+      </c>
+      <c r="Q12">
         <f>VLOOKUP(B12, references!$A$4:'references'!$G$12,7)</f>
         <v>435.75299999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R12">
+        <f t="shared" si="1"/>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>20201202</v>
       </c>
@@ -1678,19 +1786,31 @@
         <f>L2*1.3</f>
         <v>838.5</v>
       </c>
-      <c r="N13" s="2">
+      <c r="M13" s="2">
+        <f>M2*5</f>
+        <v>25</v>
+      </c>
+      <c r="N13">
+        <f>LOG10(L13)</f>
+        <v>2.9235030669421045</v>
+      </c>
+      <c r="O13" s="2">
         <v>5</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <f t="shared" si="0"/>
-        <v>3.0892739377281955</v>
-      </c>
-      <c r="P13">
+        <v>308.92739377281953</v>
+      </c>
+      <c r="Q13">
         <f>VLOOKUP(B13, references!$A$4:'references'!$G$12,7)</f>
         <v>271.423</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>2.9815146094215863</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>20201202</v>
       </c>
@@ -1725,22 +1845,34 @@
         <v>148</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" ref="L14:L34" si="1">L3*1.3</f>
+        <f t="shared" ref="L14:L34" si="2">L3*1.3</f>
         <v>1866.8</v>
       </c>
-      <c r="N14" s="2">
+      <c r="M14" s="2">
+        <f t="shared" ref="M14:M34" si="3">M3*5</f>
+        <v>60</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ref="N14:N34" si="4">LOG10(L14)</f>
+        <v>3.2710977922131184</v>
+      </c>
+      <c r="O14" s="2">
         <v>9</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <f t="shared" si="0"/>
-        <v>4.2840783654960495</v>
-      </c>
-      <c r="P14">
+        <v>428.40783654960495</v>
+      </c>
+      <c r="Q14">
         <f>VLOOKUP(B14, references!$A$4:'references'!$G$12,7)</f>
         <v>435.75299999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R14">
+        <f t="shared" si="1"/>
+        <v>3.2140561388472251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>20201202</v>
       </c>
@@ -1775,22 +1907,34 @@
         <v>20</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3207.1</v>
       </c>
-      <c r="N15" s="2">
+      <c r="M15" s="2">
+        <f t="shared" si="3"/>
+        <v>125</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>3.5061125017965726</v>
+      </c>
+      <c r="O15" s="2">
         <v>1</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <f t="shared" si="0"/>
-        <v>5.2135421069401184</v>
-      </c>
-      <c r="P15">
+        <v>521.35421069401184</v>
+      </c>
+      <c r="Q15">
         <f>VLOOKUP(B15, references!$A$4:'references'!$G$12,7)</f>
         <v>615.14800000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>3.8976021951295561</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>20201202</v>
       </c>
@@ -1825,22 +1969,34 @@
         <v>32</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5090.8</v>
       </c>
-      <c r="N16" s="2">
+      <c r="M16" s="2">
+        <f t="shared" si="3"/>
+        <v>440</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>3.7067860354379372</v>
+      </c>
+      <c r="O16" s="2">
         <v>8</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <f t="shared" si="0"/>
-        <v>28.995346664920003</v>
-      </c>
-      <c r="P16">
+        <v>2899.5346664920003</v>
+      </c>
+      <c r="Q16">
         <f>VLOOKUP(B16, references!$A$4:'references'!$G$12,7)</f>
         <v>175.57300000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R16">
+        <f t="shared" si="1"/>
+        <v>8.6430423509075194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>20201202</v>
       </c>
@@ -1875,22 +2031,34 @@
         <v>16</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2550.6</v>
       </c>
-      <c r="N17" s="2">
+      <c r="M17" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="4"/>
+        <v>3.4066423553507663</v>
+      </c>
+      <c r="O17" s="2">
         <v>4</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <f t="shared" si="0"/>
-        <v>5.1555498060554363</v>
-      </c>
-      <c r="P17">
+        <v>515.55498060554362</v>
+      </c>
+      <c r="Q17">
         <f>VLOOKUP(B17, references!$A$4:'references'!$G$12,7)</f>
         <v>494.72899999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>0.98016153062024625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>20201202</v>
       </c>
@@ -1925,22 +2093,34 @@
         <v>2</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1150.5</v>
       </c>
-      <c r="N18" s="2">
+      <c r="M18" s="2">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="4"/>
+        <v>3.0608866230046621</v>
+      </c>
+      <c r="O18" s="2">
         <v>2</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <f t="shared" si="0"/>
-        <v>5.1713908142075029</v>
-      </c>
-      <c r="P18">
+        <v>517.13908142075024</v>
+      </c>
+      <c r="Q18">
         <f>VLOOKUP(B18, references!$A$4:'references'!$G$12,7)</f>
         <v>222.47399999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R18">
+        <f t="shared" si="1"/>
+        <v>8.6918730986527599</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>20201202</v>
       </c>
@@ -1975,22 +2155,34 @@
         <v>0</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1227.2</v>
       </c>
-      <c r="N19" s="2">
+      <c r="M19" s="2">
+        <f t="shared" si="3"/>
+        <v>125</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="4"/>
+        <v>3.0889153466049057</v>
+      </c>
+      <c r="O19" s="2">
         <v>7</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <f t="shared" si="0"/>
-        <v>6.98968520216662</v>
-      </c>
-      <c r="P19">
+        <v>698.968520216662</v>
+      </c>
+      <c r="Q19">
         <f>VLOOKUP(B19, references!$A$4:'references'!$G$12,7)</f>
         <v>175.57300000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R19">
+        <f t="shared" si="1"/>
+        <v>10.185788787483704</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>20201202</v>
       </c>
@@ -2025,22 +2217,34 @@
         <v>1</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1333.8</v>
       </c>
-      <c r="N20" s="2">
+      <c r="M20" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="4"/>
+        <v>3.1250907130826344</v>
+      </c>
+      <c r="O20" s="2">
         <v>6</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <f t="shared" si="0"/>
-        <v>3.2652201906058207</v>
-      </c>
-      <c r="P20">
+        <v>326.52201906058207</v>
+      </c>
+      <c r="Q20">
         <f>VLOOKUP(B20, references!$A$4:'references'!$G$12,7)</f>
         <v>408.48700000000002</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R20">
+        <f t="shared" si="1"/>
+        <v>1.4994751836857101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20201202</v>
       </c>
@@ -2075,22 +2279,34 @@
         <v>6</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1567.8</v>
       </c>
-      <c r="N21" s="2">
+      <c r="M21" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="4"/>
+        <v>3.1952906601109694</v>
+      </c>
+      <c r="O21" s="2">
         <v>3</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <f t="shared" si="0"/>
-        <v>2.4273370357009596</v>
-      </c>
-      <c r="P21">
+        <v>242.73370357009597</v>
+      </c>
+      <c r="Q21">
         <f>VLOOKUP(B21, references!$A$4:'references'!$G$12,7)</f>
         <v>645.89300000000003</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R21">
+        <f t="shared" si="1"/>
+        <v>0.31891822936599057</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20201202</v>
       </c>
@@ -2125,22 +2341,34 @@
         <v>0</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63.7</v>
       </c>
+      <c r="M22" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
       <c r="N22">
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1.8041394323353503</v>
       </c>
       <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="0"/>
-        <v>0.2346890278274133</v>
-      </c>
-      <c r="P22">
+        <v>23.468902782741331</v>
+      </c>
+      <c r="Q22">
         <f>VLOOKUP(B22, references!$A$4:'references'!$G$12,7)</f>
         <v>271.423</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R22">
+        <f t="shared" si="1"/>
+        <v>15.698587127158556</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>20201202</v>
       </c>
@@ -2175,22 +2403,33 @@
         <v>0</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41.6</v>
       </c>
+      <c r="M23" s="2">
+        <v>4</v>
+      </c>
       <c r="N23">
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1.6190933306267428</v>
       </c>
       <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="0"/>
-        <v>9.5466927364814477E-2</v>
-      </c>
-      <c r="P23">
+        <v>9.5466927364814484</v>
+      </c>
+      <c r="Q23">
         <f>VLOOKUP(B23, references!$A$4:'references'!$G$12,7)</f>
         <v>435.75299999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R23">
+        <f t="shared" si="1"/>
+        <v>9.615384615384615</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>20201203</v>
       </c>
@@ -2228,19 +2467,31 @@
         <f>L13*1.3</f>
         <v>1090.05</v>
       </c>
-      <c r="N24" s="2">
+      <c r="M24" s="2">
+        <f>M13*5</f>
+        <v>125</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="4"/>
+        <v>3.0374464192489414</v>
+      </c>
+      <c r="O24" s="2">
         <v>5</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <f t="shared" si="0"/>
-        <v>4.0160561190466542</v>
-      </c>
-      <c r="P24">
+        <v>401.60561190466541</v>
+      </c>
+      <c r="Q24">
         <f>VLOOKUP(B24, references!$A$4:'references'!$G$12,7)</f>
         <v>271.423</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R24">
+        <f t="shared" si="1"/>
+        <v>11.467363882390716</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>20201203</v>
       </c>
@@ -2275,22 +2526,34 @@
         <v>148</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2426.84</v>
       </c>
-      <c r="N25" s="2">
+      <c r="M25" s="2">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="4"/>
+        <v>3.3850411445199553</v>
+      </c>
+      <c r="O25" s="2">
         <v>9</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <f t="shared" si="0"/>
-        <v>5.5693018751448644</v>
-      </c>
-      <c r="P25">
+        <v>556.93018751448642</v>
+      </c>
+      <c r="Q25">
         <f>VLOOKUP(B25, references!$A$4:'references'!$G$12,7)</f>
         <v>435.75299999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R25">
+        <f t="shared" si="1"/>
+        <v>12.361754380181635</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>20201203</v>
       </c>
@@ -2325,22 +2588,34 @@
         <v>20</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4169.2300000000005</v>
       </c>
-      <c r="N26" s="2">
+      <c r="M26" s="2">
+        <f t="shared" si="3"/>
+        <v>625</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="4"/>
+        <v>3.6200558541034096</v>
+      </c>
+      <c r="O26" s="2">
         <v>1</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <f t="shared" si="0"/>
-        <v>6.7776047390221548</v>
-      </c>
-      <c r="P26">
+        <v>677.76047390221549</v>
+      </c>
+      <c r="Q26">
         <f>VLOOKUP(B26, references!$A$4:'references'!$G$12,7)</f>
         <v>615.14800000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R26">
+        <f t="shared" si="1"/>
+        <v>14.990777673575215</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>20201203</v>
       </c>
@@ -2375,22 +2650,34 @@
         <v>32</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6618.0400000000009</v>
       </c>
-      <c r="N27" s="2">
+      <c r="M27" s="2">
+        <f t="shared" si="3"/>
+        <v>2200</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="4"/>
+        <v>3.8207293877447737</v>
+      </c>
+      <c r="O27" s="2">
         <v>8</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <f t="shared" si="0"/>
-        <v>37.693950664396013</v>
-      </c>
-      <c r="P27">
+        <v>3769.3950664396011</v>
+      </c>
+      <c r="Q27">
         <f>VLOOKUP(B27, references!$A$4:'references'!$G$12,7)</f>
         <v>175.57300000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R27">
+        <f t="shared" si="1"/>
+        <v>33.242470580413531</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>20201203</v>
       </c>
@@ -2425,22 +2712,34 @@
         <v>16</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3315.78</v>
       </c>
-      <c r="N28" s="2">
+      <c r="M28" s="2">
+        <f t="shared" si="3"/>
+        <v>125</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="4"/>
+        <v>3.5205857076576033</v>
+      </c>
+      <c r="O28" s="2">
         <v>4</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <f t="shared" si="0"/>
-        <v>6.7022147478720679</v>
-      </c>
-      <c r="P28">
+        <v>670.22147478720683</v>
+      </c>
+      <c r="Q28">
         <f>VLOOKUP(B28, references!$A$4:'references'!$G$12,7)</f>
         <v>494.72899999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R28">
+        <f t="shared" si="1"/>
+        <v>3.7698520408471006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>20201203</v>
       </c>
@@ -2475,22 +2774,34 @@
         <v>2</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1495.65</v>
       </c>
-      <c r="N29" s="2">
+      <c r="M29" s="2">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="4"/>
+        <v>3.174829975311499</v>
+      </c>
+      <c r="O29" s="2">
         <v>2</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <f t="shared" si="0"/>
-        <v>6.7228080584697549</v>
-      </c>
-      <c r="P29">
+        <v>672.28080584697545</v>
+      </c>
+      <c r="Q29">
         <f>VLOOKUP(B29, references!$A$4:'references'!$G$12,7)</f>
         <v>222.47399999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R29">
+        <f t="shared" si="1"/>
+        <v>33.430281148664456</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>20201203</v>
       </c>
@@ -2525,22 +2836,34 @@
         <v>0</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1595.3600000000001</v>
       </c>
-      <c r="N30" s="2">
+      <c r="M30" s="2">
+        <f t="shared" si="3"/>
+        <v>625</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="4"/>
+        <v>3.2028586989117427</v>
+      </c>
+      <c r="O30" s="2">
         <v>7</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <f t="shared" si="0"/>
-        <v>9.0865907628166074</v>
-      </c>
-      <c r="P30">
+        <v>908.65907628166076</v>
+      </c>
+      <c r="Q30">
         <f>VLOOKUP(B30, references!$A$4:'references'!$G$12,7)</f>
         <v>175.57300000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R30">
+        <f t="shared" si="1"/>
+        <v>39.176110721091163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>20201203</v>
       </c>
@@ -2575,22 +2898,34 @@
         <v>1</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1733.94</v>
       </c>
-      <c r="N31" s="2">
+      <c r="M31" s="2">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="4"/>
+        <v>3.2390340653894709</v>
+      </c>
+      <c r="O31" s="2">
         <v>6</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <f t="shared" si="0"/>
-        <v>4.2447862477875669</v>
-      </c>
-      <c r="P31">
+        <v>424.47862477875668</v>
+      </c>
+      <c r="Q31">
         <f>VLOOKUP(B31, references!$A$4:'references'!$G$12,7)</f>
         <v>408.48700000000002</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R31">
+        <f t="shared" si="1"/>
+        <v>5.7672122449450383</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>20201203</v>
       </c>
@@ -2625,22 +2960,34 @@
         <v>6</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2038.14</v>
       </c>
-      <c r="N32" s="2">
+      <c r="M32" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="4"/>
+        <v>3.3092340124178059</v>
+      </c>
+      <c r="O32" s="2">
         <v>3</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <f t="shared" si="0"/>
-        <v>3.1555381464112475</v>
-      </c>
-      <c r="P32">
+        <v>315.55381464112475</v>
+      </c>
+      <c r="Q32">
         <f>VLOOKUP(B32, references!$A$4:'references'!$G$12,7)</f>
         <v>645.89300000000003</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R32">
+        <f t="shared" si="1"/>
+        <v>1.2266085744845789</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>20201203</v>
       </c>
@@ -2675,22 +3022,34 @@
         <v>0</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>82.81</v>
       </c>
+      <c r="M33" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
       <c r="N33">
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1.9180827846421873</v>
       </c>
       <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
         <f t="shared" si="0"/>
-        <v>0.30509573617563729</v>
-      </c>
-      <c r="P33">
+        <v>30.509573617563728</v>
+      </c>
+      <c r="Q33">
         <f>VLOOKUP(B33, references!$A$4:'references'!$G$12,7)</f>
         <v>271.423</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R33">
+        <f t="shared" si="1"/>
+        <v>60.37918125830214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>20201203</v>
       </c>
@@ -2725,19 +3084,30 @@
         <v>0</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54.080000000000005</v>
       </c>
+      <c r="M34" s="2">
+        <v>30</v>
+      </c>
       <c r="N34">
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1.7330366829335795</v>
       </c>
       <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
         <f t="shared" si="0"/>
-        <v>0.12410700557425883</v>
-      </c>
-      <c r="P34">
+        <v>12.410700557425884</v>
+      </c>
+      <c r="Q34">
         <f>VLOOKUP(B34, references!$A$4:'references'!$G$12,7)</f>
         <v>435.75299999999999</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="1"/>
+        <v>55.473372781065081</v>
       </c>
     </row>
   </sheetData>
@@ -2766,15 +3136,15 @@
       <c r="C1" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="15">
+      <c r="D1" s="13">
         <v>44181.393055555556</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -2794,8 +3164,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="6" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
adding daily Cases Bar Plot Functionality
</commit_message>
<xml_diff>
--- a/CovidBali/testingDash/plotly apps-dash-oil-and-gas/data/regencyCasesBali.xlsx
+++ b/CovidBali/testingDash/plotly apps-dash-oil-and-gas/data/regencyCasesBali.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansve\Coding\Projects-WebScraping\CovidBali\testingDash\plotly apps-dash-oil-and-gas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F48FD2-BCDC-4839-8DC6-0E88C10C7578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658DCC7E-FCEB-47E8-900E-770E61735756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="504" yWindow="312" windowWidth="21612" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="504" yWindow="312" windowWidth="21612" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -708,13 +708,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1020,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1154,8 +1154,8 @@
         <v>0.77519379844961245</v>
       </c>
       <c r="S2">
-        <f>Q2/M2</f>
-        <v>54.284599999999998</v>
+        <f>M2/Q2*100</f>
+        <v>1.8421430755683932</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -1216,6 +1216,10 @@
         <f t="shared" ref="R3:R34" si="1">M3/L3*100</f>
         <v>0.83565459610027859</v>
       </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S34" si="2">M3/Q3*100</f>
+        <v>2.753853673985033</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
@@ -1275,6 +1279,10 @@
         <f t="shared" si="1"/>
         <v>1.0133765707336846</v>
       </c>
+      <c r="S4">
+        <f t="shared" si="2"/>
+        <v>4.0640626320820354</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
@@ -1313,7 +1321,7 @@
       <c r="L5" s="2">
         <v>3916</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="14">
         <v>88</v>
       </c>
       <c r="N5">
@@ -1334,6 +1342,10 @@
         <f t="shared" si="1"/>
         <v>2.2471910112359552</v>
       </c>
+      <c r="S5">
+        <f t="shared" si="2"/>
+        <v>50.12160184082974</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
@@ -1372,7 +1384,7 @@
       <c r="L6" s="2">
         <v>1962</v>
       </c>
-      <c r="M6" s="16">
+      <c r="M6" s="14">
         <v>5</v>
       </c>
       <c r="N6">
@@ -1393,6 +1405,10 @@
         <f t="shared" si="1"/>
         <v>0.254841997961264</v>
       </c>
+      <c r="S6">
+        <f t="shared" si="2"/>
+        <v>1.0106543178184422</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
@@ -1431,7 +1447,7 @@
       <c r="L7" s="2">
         <v>885</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="14">
         <v>20</v>
       </c>
       <c r="N7">
@@ -1452,6 +1468,10 @@
         <f t="shared" si="1"/>
         <v>2.2598870056497176</v>
       </c>
+      <c r="S7">
+        <f t="shared" si="2"/>
+        <v>8.9898145401260372</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
@@ -1490,7 +1510,7 @@
       <c r="L8" s="2">
         <v>944</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="14">
         <v>25</v>
       </c>
       <c r="N8">
@@ -1511,6 +1531,10 @@
         <f t="shared" si="1"/>
         <v>2.6483050847457625</v>
       </c>
+      <c r="S8">
+        <f t="shared" si="2"/>
+        <v>14.239091432053902</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
@@ -1549,7 +1573,7 @@
       <c r="L9" s="2">
         <v>1026</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="14">
         <v>4</v>
       </c>
       <c r="N9">
@@ -1570,6 +1594,10 @@
         <f t="shared" si="1"/>
         <v>0.38986354775828458</v>
       </c>
+      <c r="S9">
+        <f t="shared" si="2"/>
+        <v>0.97922332901659048</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
@@ -1608,7 +1636,7 @@
       <c r="L10" s="2">
         <v>1206</v>
       </c>
-      <c r="M10" s="16">
+      <c r="M10" s="14">
         <v>1</v>
       </c>
       <c r="N10">
@@ -1629,6 +1657,10 @@
         <f t="shared" si="1"/>
         <v>8.2918739635157543E-2</v>
       </c>
+      <c r="S10">
+        <f t="shared" si="2"/>
+        <v>0.15482440590004845</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
@@ -1667,7 +1699,7 @@
       <c r="L11" s="2">
         <v>49</v>
       </c>
-      <c r="M11" s="16">
+      <c r="M11" s="14">
         <v>2</v>
       </c>
       <c r="N11">
@@ -1688,6 +1720,10 @@
         <f t="shared" si="1"/>
         <v>4.0816326530612246</v>
       </c>
+      <c r="S11">
+        <f t="shared" si="2"/>
+        <v>0.73685723022735727</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
@@ -1726,7 +1762,7 @@
       <c r="L12" s="2">
         <v>32</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M12" s="14">
         <v>10</v>
       </c>
       <c r="N12">
@@ -1747,6 +1783,10 @@
         <f t="shared" si="1"/>
         <v>31.25</v>
       </c>
+      <c r="S12">
+        <f t="shared" si="2"/>
+        <v>2.2948780616541939</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
@@ -1809,6 +1849,10 @@
         <f t="shared" si="1"/>
         <v>2.9815146094215863</v>
       </c>
+      <c r="S13">
+        <f t="shared" si="2"/>
+        <v>9.2107153778419661</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
@@ -1845,15 +1889,15 @@
         <v>148</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" ref="L14:L34" si="2">L3*1.3</f>
+        <f t="shared" ref="L14:L34" si="3">L3*1.3</f>
         <v>1866.8</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" ref="M14:M34" si="3">M3*5</f>
+        <f t="shared" ref="M14:M33" si="4">M3*5</f>
         <v>60</v>
       </c>
       <c r="N14">
-        <f t="shared" ref="N14:N34" si="4">LOG10(L14)</f>
+        <f t="shared" ref="N14:N34" si="5">LOG10(L14)</f>
         <v>3.2710977922131184</v>
       </c>
       <c r="O14" s="2">
@@ -1871,6 +1915,10 @@
         <f t="shared" si="1"/>
         <v>3.2140561388472251</v>
       </c>
+      <c r="S14">
+        <f t="shared" si="2"/>
+        <v>13.769268369925165</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
@@ -1907,15 +1955,15 @@
         <v>20</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3207.1</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
       <c r="N15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.5061125017965726</v>
       </c>
       <c r="O15" s="2">
@@ -1933,6 +1981,10 @@
         <f t="shared" si="1"/>
         <v>3.8976021951295561</v>
       </c>
+      <c r="S15">
+        <f t="shared" si="2"/>
+        <v>20.320313160410176</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
@@ -1969,15 +2021,15 @@
         <v>32</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5090.8</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>440</v>
       </c>
       <c r="N16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.7067860354379372</v>
       </c>
       <c r="O16" s="2">
@@ -1995,8 +2047,12 @@
         <f t="shared" si="1"/>
         <v>8.6430423509075194</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S16">
+        <f t="shared" si="2"/>
+        <v>250.60800920414869</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>20201202</v>
       </c>
@@ -2031,15 +2087,15 @@
         <v>16</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2550.6</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="N17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.4066423553507663</v>
       </c>
       <c r="O17" s="2">
@@ -2057,8 +2113,12 @@
         <f t="shared" si="1"/>
         <v>0.98016153062024625</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S17">
+        <f t="shared" si="2"/>
+        <v>5.0532715890922102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>20201202</v>
       </c>
@@ -2093,15 +2153,15 @@
         <v>2</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1150.5</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.0608866230046621</v>
       </c>
       <c r="O18" s="2">
@@ -2119,8 +2179,12 @@
         <f t="shared" si="1"/>
         <v>8.6918730986527599</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S18">
+        <f t="shared" si="2"/>
+        <v>44.94907270063019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>20201202</v>
       </c>
@@ -2155,15 +2219,15 @@
         <v>0</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1227.2</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
       <c r="N19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.0889153466049057</v>
       </c>
       <c r="O19" s="2">
@@ -2181,8 +2245,12 @@
         <f t="shared" si="1"/>
         <v>10.185788787483704</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S19">
+        <f t="shared" si="2"/>
+        <v>71.195457160269513</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>20201202</v>
       </c>
@@ -2217,15 +2285,15 @@
         <v>1</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1333.8</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="N20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.1250907130826344</v>
       </c>
       <c r="O20" s="2">
@@ -2243,8 +2311,12 @@
         <f t="shared" si="1"/>
         <v>1.4994751836857101</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S20">
+        <f t="shared" si="2"/>
+        <v>4.8961166450829516</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20201202</v>
       </c>
@@ -2279,15 +2351,15 @@
         <v>6</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1567.8</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="N21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.1952906601109694</v>
       </c>
       <c r="O21" s="2">
@@ -2305,8 +2377,12 @@
         <f t="shared" si="1"/>
         <v>0.31891822936599057</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S21">
+        <f t="shared" si="2"/>
+        <v>0.77412202950024223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20201202</v>
       </c>
@@ -2341,15 +2417,15 @@
         <v>0</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>63.7</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="N22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.8041394323353503</v>
       </c>
       <c r="O22">
@@ -2367,8 +2443,12 @@
         <f t="shared" si="1"/>
         <v>15.698587127158556</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S22">
+        <f t="shared" si="2"/>
+        <v>3.6842861511367864</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>20201202</v>
       </c>
@@ -2403,14 +2483,14 @@
         <v>0</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41.6</v>
       </c>
       <c r="M23" s="2">
         <v>4</v>
       </c>
       <c r="N23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.6190933306267428</v>
       </c>
       <c r="O23">
@@ -2428,8 +2508,12 @@
         <f t="shared" si="1"/>
         <v>9.615384615384615</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S23">
+        <f t="shared" si="2"/>
+        <v>0.91795122466167767</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>20201203</v>
       </c>
@@ -2472,7 +2556,7 @@
         <v>125</v>
       </c>
       <c r="N24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.0374464192489414</v>
       </c>
       <c r="O24" s="2">
@@ -2490,8 +2574,12 @@
         <f t="shared" si="1"/>
         <v>11.467363882390716</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S24">
+        <f t="shared" si="2"/>
+        <v>46.053576889209829</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>20201203</v>
       </c>
@@ -2526,15 +2614,15 @@
         <v>148</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2426.84</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="N25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.3850411445199553</v>
       </c>
       <c r="O25" s="2">
@@ -2552,8 +2640,12 @@
         <f t="shared" si="1"/>
         <v>12.361754380181635</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S25">
+        <f t="shared" si="2"/>
+        <v>68.84634184962583</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>20201203</v>
       </c>
@@ -2588,15 +2680,15 @@
         <v>20</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4169.2300000000005</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>625</v>
       </c>
       <c r="N26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.6200558541034096</v>
       </c>
       <c r="O26" s="2">
@@ -2614,8 +2706,12 @@
         <f t="shared" si="1"/>
         <v>14.990777673575215</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S26">
+        <f t="shared" si="2"/>
+        <v>101.60156580205089</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>20201203</v>
       </c>
@@ -2650,15 +2746,15 @@
         <v>32</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6618.0400000000009</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2200</v>
       </c>
       <c r="N27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8207293877447737</v>
       </c>
       <c r="O27" s="2">
@@ -2676,8 +2772,12 @@
         <f t="shared" si="1"/>
         <v>33.242470580413531</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S27">
+        <f t="shared" si="2"/>
+        <v>1253.0400460207436</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>20201203</v>
       </c>
@@ -2712,15 +2812,15 @@
         <v>16</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3315.78</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125</v>
       </c>
       <c r="N28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.5205857076576033</v>
       </c>
       <c r="O28" s="2">
@@ -2738,8 +2838,12 @@
         <f t="shared" si="1"/>
         <v>3.7698520408471006</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S28">
+        <f t="shared" si="2"/>
+        <v>25.266357945461049</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>20201203</v>
       </c>
@@ -2774,15 +2878,15 @@
         <v>2</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1495.65</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>500</v>
       </c>
       <c r="N29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.174829975311499</v>
       </c>
       <c r="O29" s="2">
@@ -2800,8 +2904,12 @@
         <f t="shared" si="1"/>
         <v>33.430281148664456</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S29">
+        <f t="shared" si="2"/>
+        <v>224.74536350315094</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>20201203</v>
       </c>
@@ -2836,15 +2944,15 @@
         <v>0</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1595.3600000000001</v>
       </c>
       <c r="M30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>625</v>
       </c>
       <c r="N30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.2028586989117427</v>
       </c>
       <c r="O30" s="2">
@@ -2862,8 +2970,12 @@
         <f t="shared" si="1"/>
         <v>39.176110721091163</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S30">
+        <f t="shared" si="2"/>
+        <v>355.97728580134753</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>20201203</v>
       </c>
@@ -2898,15 +3010,15 @@
         <v>1</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1733.94</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="N31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.2390340653894709</v>
       </c>
       <c r="O31" s="2">
@@ -2924,8 +3036,12 @@
         <f t="shared" si="1"/>
         <v>5.7672122449450383</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S31">
+        <f t="shared" si="2"/>
+        <v>24.480583225414762</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>20201203</v>
       </c>
@@ -2960,15 +3076,15 @@
         <v>6</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2038.14</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="N32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.3092340124178059</v>
       </c>
       <c r="O32" s="2">
@@ -2986,8 +3102,12 @@
         <f t="shared" si="1"/>
         <v>1.2266085744845789</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S32">
+        <f t="shared" si="2"/>
+        <v>3.8706101475012114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>20201203</v>
       </c>
@@ -3022,15 +3142,15 @@
         <v>0</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.81</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="N33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9180827846421873</v>
       </c>
       <c r="O33">
@@ -3048,8 +3168,12 @@
         <f t="shared" si="1"/>
         <v>60.37918125830214</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S33">
+        <f t="shared" si="2"/>
+        <v>18.421430755683932</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>20201203</v>
       </c>
@@ -3084,14 +3208,14 @@
         <v>0</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>54.080000000000005</v>
       </c>
       <c r="M34" s="2">
         <v>30</v>
       </c>
       <c r="N34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.7330366829335795</v>
       </c>
       <c r="O34">
@@ -3108,6 +3232,10 @@
       <c r="R34">
         <f t="shared" si="1"/>
         <v>55.473372781065081</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="2"/>
+        <v>6.8846341849625823</v>
       </c>
     </row>
   </sheetData>
@@ -3141,10 +3269,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -3164,8 +3292,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="6" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
scrapy spider task scheduler
</commit_message>
<xml_diff>
--- a/CovidBali/testingDash/plotly apps-dash-oil-and-gas/data/regencyCasesBali.xlsx
+++ b/CovidBali/testingDash/plotly apps-dash-oil-and-gas/data/regencyCasesBali.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansve\Coding\Projects-WebScraping\CovidBali\testingDash\plotly apps-dash-oil-and-gas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B95A8AC-0161-40AB-A532-0C2C33B60BB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3B7D66-A9B2-4C8F-900E-200D966519DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="21612" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1560" windowWidth="21612" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -686,14 +686,8 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -726,7 +720,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1030,88 +1032,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
     <col min="3" max="16" width="15" customWidth="1"/>
     <col min="17" max="17" width="15.88671875" customWidth="1"/>
     <col min="18" max="18" width="14.5546875" customWidth="1"/>
     <col min="19" max="19" width="15.44140625" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:21" s="15" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>20201201</v>
       </c>
       <c r="B2" t="s">
@@ -1120,43 +1125,43 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
         <v>26</v>
       </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
         <v>11</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>5</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>608</v>
       </c>
-      <c r="J2" s="2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
         <v>5</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>645</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>5</v>
       </c>
       <c r="O2">
         <v>2.809559714635268</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <v>5</v>
       </c>
       <c r="Q2">
@@ -1177,7 +1182,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>20201201</v>
       </c>
       <c r="B3" t="s">
@@ -1186,43 +1191,43 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
         <v>21</v>
       </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
         <v>8</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>148</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>1407</v>
       </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
         <v>148</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="1">
         <v>1436</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <v>12</v>
       </c>
       <c r="O3">
         <v>3.157154439906281</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="1">
         <v>9</v>
       </c>
       <c r="Q3">
@@ -1243,7 +1248,7 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>20201201</v>
       </c>
       <c r="B4" t="s">
@@ -1252,43 +1257,43 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
         <v>27</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>-3</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>4</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>23</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>2436</v>
       </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
         <v>20</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <v>2467</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
         <v>25</v>
       </c>
       <c r="O4">
         <v>3.3921691494897361</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="1">
         <v>1</v>
       </c>
       <c r="Q4">
@@ -1309,7 +1314,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>20201201</v>
       </c>
       <c r="B5" t="s">
@@ -1318,43 +1323,43 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
         <v>48</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
         <v>22</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>32</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>3846</v>
       </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
         <v>32</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="1">
         <v>3916</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="12">
         <v>88</v>
       </c>
       <c r="O5">
         <v>3.5928426831310998</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="1">
         <v>8</v>
       </c>
       <c r="Q5">
@@ -1375,7 +1380,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>20201201</v>
       </c>
       <c r="B6" t="s">
@@ -1384,43 +1389,43 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
         <v>29</v>
       </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
         <v>10</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>16</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>1923</v>
       </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
         <v>16</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="1">
         <v>1962</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="12">
         <v>5</v>
       </c>
       <c r="O6">
         <v>3.2926990030439298</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="1">
         <v>4</v>
       </c>
       <c r="Q6">
@@ -1441,7 +1446,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>20201201</v>
       </c>
       <c r="B7" t="s">
@@ -1450,43 +1455,43 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
         <v>58</v>
       </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
         <v>3</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>2</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>824</v>
       </c>
-      <c r="J7" s="2">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
         <v>2</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="1">
         <v>885</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="12">
         <v>20</v>
       </c>
       <c r="O7">
         <v>2.946943270697826</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="1">
         <v>2</v>
       </c>
       <c r="Q7">
@@ -1507,7 +1512,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>20201201</v>
       </c>
       <c r="B8" t="s">
@@ -1516,43 +1521,43 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
         <v>19</v>
       </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
         <v>925</v>
       </c>
-      <c r="J8" s="2">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
-        <v>0</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2">
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
         <v>944</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="12">
         <v>25</v>
       </c>
       <c r="O8">
         <v>2.9749719942980688</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="1">
         <v>7</v>
       </c>
       <c r="Q8">
@@ -1573,7 +1578,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>20201201</v>
       </c>
       <c r="B9" t="s">
@@ -1582,43 +1587,43 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
         <v>23</v>
       </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>1003</v>
       </c>
-      <c r="J9" s="2">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
         <v>1</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="1">
         <v>1026</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="12">
         <v>4</v>
       </c>
       <c r="O9">
         <v>3.011147360775797</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="1">
         <v>6</v>
       </c>
       <c r="Q9">
@@ -1639,7 +1644,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>20201201</v>
       </c>
       <c r="B10" t="s">
@@ -1648,43 +1653,43 @@
       <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
         <v>41</v>
       </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
         <v>6</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>6</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <v>1159</v>
       </c>
-      <c r="J10" s="2">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2">
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
         <v>6</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="1">
         <v>1206</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="12">
         <v>1</v>
       </c>
       <c r="O10">
         <v>3.081347307804132</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="1">
         <v>3</v>
       </c>
       <c r="Q10">
@@ -1705,7 +1710,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>20201201</v>
       </c>
       <c r="B11" t="s">
@@ -1714,37 +1719,37 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
         <v>5</v>
       </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
         <v>31</v>
       </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
         <v>13</v>
       </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0</v>
-      </c>
-      <c r="M11" s="2">
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
         <v>49</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11" s="12">
         <v>2</v>
       </c>
       <c r="O11">
@@ -1771,7 +1776,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>20201201</v>
       </c>
       <c r="B12" t="s">
@@ -1780,37 +1785,37 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
         <v>8</v>
       </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
         <v>2</v>
       </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
         <v>22</v>
       </c>
-      <c r="J12" s="2">
-        <v>0</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0</v>
-      </c>
-      <c r="M12" s="2">
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
         <v>32</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="12">
         <v>10</v>
       </c>
       <c r="O12">
@@ -1837,7 +1842,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>20201202</v>
       </c>
       <c r="B13" t="s">
@@ -1846,38 +1851,38 @@
       <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
         <v>26</v>
       </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
         <v>11</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <v>5</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>608</v>
       </c>
-      <c r="J13" s="2">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2">
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
         <v>5</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="1">
         <f>M2*1.3</f>
         <v>838.5</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="1">
         <f>N2*5</f>
         <v>25</v>
       </c>
@@ -1885,7 +1890,7 @@
         <f>LOG10(M13)</f>
         <v>2.9235030669421045</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="1">
         <v>5</v>
       </c>
       <c r="Q13">
@@ -1906,7 +1911,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>20201202</v>
       </c>
       <c r="B14" t="s">
@@ -1915,38 +1920,38 @@
       <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
         <v>21</v>
       </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
         <v>8</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <v>148</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <v>1407</v>
       </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <v>0</v>
-      </c>
-      <c r="L14" s="2">
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
         <v>148</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="1">
         <f t="shared" ref="M14:M34" si="3">M3*1.3</f>
         <v>1866.8</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="1">
         <f t="shared" ref="N14:N33" si="4">N3*5</f>
         <v>60</v>
       </c>
@@ -1954,7 +1959,7 @@
         <f t="shared" ref="O14:O34" si="5">LOG10(M14)</f>
         <v>3.2710977922131184</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="1">
         <v>9</v>
       </c>
       <c r="Q14">
@@ -1975,7 +1980,7 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>20201202</v>
       </c>
       <c r="B15" t="s">
@@ -1984,38 +1989,38 @@
       <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
         <v>27</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>-3</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>4</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <v>23</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <v>2436</v>
       </c>
-      <c r="J15" s="2">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2">
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
         <v>20</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="1">
         <f t="shared" si="3"/>
         <v>3207.1</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="1">
         <f t="shared" si="4"/>
         <v>125</v>
       </c>
@@ -2023,7 +2028,7 @@
         <f t="shared" si="5"/>
         <v>3.5061125017965726</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="1">
         <v>1</v>
       </c>
       <c r="Q15">
@@ -2044,7 +2049,7 @@
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>20201202</v>
       </c>
       <c r="B16" t="s">
@@ -2053,38 +2058,38 @@
       <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
         <v>48</v>
       </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
         <v>22</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
         <v>32</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <v>3846</v>
       </c>
-      <c r="J16" s="2">
-        <v>0</v>
-      </c>
-      <c r="K16" s="2">
-        <v>0</v>
-      </c>
-      <c r="L16" s="2">
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
         <v>32</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="1">
         <f t="shared" si="3"/>
         <v>5090.8</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="1">
         <f t="shared" si="4"/>
         <v>440</v>
       </c>
@@ -2092,7 +2097,7 @@
         <f t="shared" si="5"/>
         <v>3.7067860354379372</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="1">
         <v>8</v>
       </c>
       <c r="Q16">
@@ -2113,7 +2118,7 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>20201202</v>
       </c>
       <c r="B17" t="s">
@@ -2122,38 +2127,38 @@
       <c r="C17" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
         <v>29</v>
       </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2">
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
         <v>10</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
         <v>16</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="1">
         <v>1923</v>
       </c>
-      <c r="J17" s="2">
-        <v>0</v>
-      </c>
-      <c r="K17" s="2">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2">
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
         <v>16</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="1">
         <f t="shared" si="3"/>
         <v>2550.6</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="1">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
@@ -2161,7 +2166,7 @@
         <f t="shared" si="5"/>
         <v>3.4066423553507663</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17" s="1">
         <v>4</v>
       </c>
       <c r="Q17">
@@ -2182,7 +2187,7 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>20201202</v>
       </c>
       <c r="B18" t="s">
@@ -2191,38 +2196,38 @@
       <c r="C18" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
         <v>58</v>
       </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2">
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
         <v>3</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
         <v>2</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="1">
         <v>824</v>
       </c>
-      <c r="J18" s="2">
-        <v>0</v>
-      </c>
-      <c r="K18" s="2">
-        <v>0</v>
-      </c>
-      <c r="L18" s="2">
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
         <v>2</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="1">
         <f t="shared" si="3"/>
         <v>1150.5</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N18" s="1">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
@@ -2230,7 +2235,7 @@
         <f t="shared" si="5"/>
         <v>3.0608866230046621</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P18" s="1">
         <v>2</v>
       </c>
       <c r="Q18">
@@ -2251,7 +2256,7 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>20201202</v>
       </c>
       <c r="B19" t="s">
@@ -2260,38 +2265,38 @@
       <c r="C19" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2">
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
         <v>19</v>
       </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2">
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
         <v>925</v>
       </c>
-      <c r="J19" s="2">
-        <v>0</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0</v>
-      </c>
-      <c r="L19" s="2">
-        <v>0</v>
-      </c>
-      <c r="M19" s="2">
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
         <f t="shared" si="3"/>
         <v>1227.2</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19" s="1">
         <f t="shared" si="4"/>
         <v>125</v>
       </c>
@@ -2299,7 +2304,7 @@
         <f t="shared" si="5"/>
         <v>3.0889153466049057</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P19" s="1">
         <v>7</v>
       </c>
       <c r="Q19">
@@ -2320,7 +2325,7 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>20201202</v>
       </c>
       <c r="B20" t="s">
@@ -2329,38 +2334,38 @@
       <c r="C20" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
         <v>23</v>
       </c>
-      <c r="F20" s="2">
-        <v>0</v>
-      </c>
-      <c r="G20" s="2">
-        <v>0</v>
-      </c>
-      <c r="H20" s="2">
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
         <v>1</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="1">
         <v>1003</v>
       </c>
-      <c r="J20" s="2">
-        <v>0</v>
-      </c>
-      <c r="K20" s="2">
-        <v>0</v>
-      </c>
-      <c r="L20" s="2">
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
         <v>1</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="1">
         <f t="shared" si="3"/>
         <v>1333.8</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N20" s="1">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
@@ -2368,7 +2373,7 @@
         <f t="shared" si="5"/>
         <v>3.1250907130826344</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P20" s="1">
         <v>6</v>
       </c>
       <c r="Q20">
@@ -2389,7 +2394,7 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>20201202</v>
       </c>
       <c r="B21" t="s">
@@ -2398,38 +2403,38 @@
       <c r="C21" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2">
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
         <v>41</v>
       </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
         <v>6</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="1">
         <v>6</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="1">
         <v>1159</v>
       </c>
-      <c r="J21" s="2">
-        <v>0</v>
-      </c>
-      <c r="K21" s="2">
-        <v>0</v>
-      </c>
-      <c r="L21" s="2">
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
         <v>6</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21" s="1">
         <f t="shared" si="3"/>
         <v>1567.8</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N21" s="1">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
@@ -2437,7 +2442,7 @@
         <f t="shared" si="5"/>
         <v>3.1952906601109694</v>
       </c>
-      <c r="P21" s="2">
+      <c r="P21" s="1">
         <v>3</v>
       </c>
       <c r="Q21">
@@ -2458,7 +2463,7 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>20201202</v>
       </c>
       <c r="B22" t="s">
@@ -2467,38 +2472,38 @@
       <c r="C22" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2">
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
         <v>5</v>
       </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2">
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
         <v>31</v>
       </c>
-      <c r="H22" s="2">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
         <v>13</v>
       </c>
-      <c r="J22" s="2">
-        <v>0</v>
-      </c>
-      <c r="K22" s="2">
-        <v>0</v>
-      </c>
-      <c r="L22" s="2">
-        <v>0</v>
-      </c>
-      <c r="M22" s="2">
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
         <f t="shared" si="3"/>
         <v>63.7</v>
       </c>
-      <c r="N22" s="2">
+      <c r="N22" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
@@ -2527,7 +2532,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>20201202</v>
       </c>
       <c r="B23" t="s">
@@ -2536,38 +2541,38 @@
       <c r="C23" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2">
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
         <v>8</v>
       </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2">
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
         <v>2</v>
       </c>
-      <c r="H23" s="2">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2">
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
         <v>22</v>
       </c>
-      <c r="J23" s="2">
-        <v>0</v>
-      </c>
-      <c r="K23" s="2">
-        <v>0</v>
-      </c>
-      <c r="L23" s="2">
-        <v>0</v>
-      </c>
-      <c r="M23" s="2">
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
         <f t="shared" si="3"/>
         <v>41.6</v>
       </c>
-      <c r="N23" s="2">
+      <c r="N23" s="1">
         <v>4</v>
       </c>
       <c r="O23">
@@ -2595,7 +2600,7 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>20201203</v>
       </c>
       <c r="B24" t="s">
@@ -2604,38 +2609,38 @@
       <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="2">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
         <v>26</v>
       </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2">
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
         <v>11</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="1">
         <v>5</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="1">
         <v>608</v>
       </c>
-      <c r="J24" s="2">
-        <v>0</v>
-      </c>
-      <c r="K24" s="2">
-        <v>0</v>
-      </c>
-      <c r="L24" s="2">
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
         <v>5</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="1">
         <f>M13*1.3</f>
         <v>1090.05</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N24" s="1">
         <f>N13*5</f>
         <v>125</v>
       </c>
@@ -2643,7 +2648,7 @@
         <f t="shared" si="5"/>
         <v>3.0374464192489414</v>
       </c>
-      <c r="P24" s="2">
+      <c r="P24" s="1">
         <v>5</v>
       </c>
       <c r="Q24">
@@ -2664,7 +2669,7 @@
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>20201203</v>
       </c>
       <c r="B25" t="s">
@@ -2673,38 +2678,38 @@
       <c r="C25" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
         <v>21</v>
       </c>
-      <c r="F25" s="2">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2">
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
         <v>8</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="1">
         <v>148</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="1">
         <v>1407</v>
       </c>
-      <c r="J25" s="2">
-        <v>0</v>
-      </c>
-      <c r="K25" s="2">
-        <v>0</v>
-      </c>
-      <c r="L25" s="2">
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
         <v>148</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="1">
         <f t="shared" si="3"/>
         <v>2426.84</v>
       </c>
-      <c r="N25" s="2">
+      <c r="N25" s="1">
         <f t="shared" si="4"/>
         <v>300</v>
       </c>
@@ -2712,7 +2717,7 @@
         <f t="shared" si="5"/>
         <v>3.3850411445199553</v>
       </c>
-      <c r="P25" s="2">
+      <c r="P25" s="1">
         <v>9</v>
       </c>
       <c r="Q25">
@@ -2733,7 +2738,7 @@
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>20201203</v>
       </c>
       <c r="B26" t="s">
@@ -2742,38 +2747,38 @@
       <c r="C26" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="2">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
         <v>27</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="1">
         <v>-3</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="1">
         <v>4</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="1">
         <v>23</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="1">
         <v>2436</v>
       </c>
-      <c r="J26" s="2">
-        <v>0</v>
-      </c>
-      <c r="K26" s="2">
-        <v>0</v>
-      </c>
-      <c r="L26" s="2">
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
         <v>20</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="1">
         <f t="shared" si="3"/>
         <v>4169.2300000000005</v>
       </c>
-      <c r="N26" s="2">
+      <c r="N26" s="1">
         <f t="shared" si="4"/>
         <v>625</v>
       </c>
@@ -2781,7 +2786,7 @@
         <f t="shared" si="5"/>
         <v>3.6200558541034096</v>
       </c>
-      <c r="P26" s="2">
+      <c r="P26" s="1">
         <v>1</v>
       </c>
       <c r="Q26">
@@ -2802,7 +2807,7 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>20201203</v>
       </c>
       <c r="B27" t="s">
@@ -2811,38 +2816,38 @@
       <c r="C27" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="2">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2">
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
         <v>48</v>
       </c>
-      <c r="F27" s="2">
-        <v>0</v>
-      </c>
-      <c r="G27" s="2">
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
         <v>22</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="1">
         <v>32</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="1">
         <v>3846</v>
       </c>
-      <c r="J27" s="2">
-        <v>0</v>
-      </c>
-      <c r="K27" s="2">
-        <v>0</v>
-      </c>
-      <c r="L27" s="2">
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
         <v>32</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27" s="1">
         <f t="shared" si="3"/>
         <v>6618.0400000000009</v>
       </c>
-      <c r="N27" s="2">
+      <c r="N27" s="1">
         <f t="shared" si="4"/>
         <v>2200</v>
       </c>
@@ -2850,7 +2855,7 @@
         <f t="shared" si="5"/>
         <v>3.8207293877447737</v>
       </c>
-      <c r="P27" s="2">
+      <c r="P27" s="1">
         <v>8</v>
       </c>
       <c r="Q27">
@@ -2871,7 +2876,7 @@
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>20201203</v>
       </c>
       <c r="B28" t="s">
@@ -2880,38 +2885,38 @@
       <c r="C28" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="2">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2">
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
         <v>29</v>
       </c>
-      <c r="F28" s="2">
-        <v>0</v>
-      </c>
-      <c r="G28" s="2">
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
         <v>10</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="1">
         <v>16</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="1">
         <v>1923</v>
       </c>
-      <c r="J28" s="2">
-        <v>0</v>
-      </c>
-      <c r="K28" s="2">
-        <v>0</v>
-      </c>
-      <c r="L28" s="2">
+      <c r="J28" s="1">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
         <v>16</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M28" s="1">
         <f t="shared" si="3"/>
         <v>3315.78</v>
       </c>
-      <c r="N28" s="2">
+      <c r="N28" s="1">
         <f t="shared" si="4"/>
         <v>125</v>
       </c>
@@ -2919,7 +2924,7 @@
         <f t="shared" si="5"/>
         <v>3.5205857076576033</v>
       </c>
-      <c r="P28" s="2">
+      <c r="P28" s="1">
         <v>4</v>
       </c>
       <c r="Q28">
@@ -2940,7 +2945,7 @@
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+      <c r="A29" s="2">
         <v>20201203</v>
       </c>
       <c r="B29" t="s">
@@ -2949,38 +2954,38 @@
       <c r="C29" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="2">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2">
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
         <v>58</v>
       </c>
-      <c r="F29" s="2">
-        <v>0</v>
-      </c>
-      <c r="G29" s="2">
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
         <v>3</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="1">
         <v>2</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="1">
         <v>824</v>
       </c>
-      <c r="J29" s="2">
-        <v>0</v>
-      </c>
-      <c r="K29" s="2">
-        <v>0</v>
-      </c>
-      <c r="L29" s="2">
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
         <v>2</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29" s="1">
         <f t="shared" si="3"/>
         <v>1495.65</v>
       </c>
-      <c r="N29" s="2">
+      <c r="N29" s="1">
         <f t="shared" si="4"/>
         <v>500</v>
       </c>
@@ -2988,7 +2993,7 @@
         <f t="shared" si="5"/>
         <v>3.174829975311499</v>
       </c>
-      <c r="P29" s="2">
+      <c r="P29" s="1">
         <v>2</v>
       </c>
       <c r="Q29">
@@ -3009,7 +3014,7 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>20201203</v>
       </c>
       <c r="B30" t="s">
@@ -3018,38 +3023,38 @@
       <c r="C30" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="2">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2">
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
         <v>19</v>
       </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
-        <v>0</v>
-      </c>
-      <c r="I30" s="2">
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
         <v>925</v>
       </c>
-      <c r="J30" s="2">
-        <v>0</v>
-      </c>
-      <c r="K30" s="2">
-        <v>0</v>
-      </c>
-      <c r="L30" s="2">
-        <v>0</v>
-      </c>
-      <c r="M30" s="2">
+      <c r="J30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
         <f t="shared" si="3"/>
         <v>1595.3600000000001</v>
       </c>
-      <c r="N30" s="2">
+      <c r="N30" s="1">
         <f t="shared" si="4"/>
         <v>625</v>
       </c>
@@ -3057,7 +3062,7 @@
         <f t="shared" si="5"/>
         <v>3.2028586989117427</v>
       </c>
-      <c r="P30" s="2">
+      <c r="P30" s="1">
         <v>7</v>
       </c>
       <c r="Q30">
@@ -3078,7 +3083,7 @@
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
+      <c r="A31" s="2">
         <v>20201203</v>
       </c>
       <c r="B31" t="s">
@@ -3087,38 +3092,38 @@
       <c r="C31" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2">
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
         <v>23</v>
       </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
         <v>1</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="1">
         <v>1003</v>
       </c>
-      <c r="J31" s="2">
-        <v>0</v>
-      </c>
-      <c r="K31" s="2">
-        <v>0</v>
-      </c>
-      <c r="L31" s="2">
+      <c r="J31" s="1">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
         <v>1</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31" s="1">
         <f t="shared" si="3"/>
         <v>1733.94</v>
       </c>
-      <c r="N31" s="2">
+      <c r="N31" s="1">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
@@ -3126,7 +3131,7 @@
         <f t="shared" si="5"/>
         <v>3.2390340653894709</v>
       </c>
-      <c r="P31" s="2">
+      <c r="P31" s="1">
         <v>6</v>
       </c>
       <c r="Q31">
@@ -3147,7 +3152,7 @@
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="3">
+      <c r="A32" s="2">
         <v>20201203</v>
       </c>
       <c r="B32" t="s">
@@ -3156,38 +3161,38 @@
       <c r="C32" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2">
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
         <v>41</v>
       </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
         <v>6</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="1">
         <v>6</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="1">
         <v>1159</v>
       </c>
-      <c r="J32" s="2">
-        <v>0</v>
-      </c>
-      <c r="K32" s="2">
-        <v>0</v>
-      </c>
-      <c r="L32" s="2">
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
         <v>6</v>
       </c>
-      <c r="M32" s="2">
+      <c r="M32" s="1">
         <f t="shared" si="3"/>
         <v>2038.14</v>
       </c>
-      <c r="N32" s="2">
+      <c r="N32" s="1">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
@@ -3195,7 +3200,7 @@
         <f t="shared" si="5"/>
         <v>3.3092340124178059</v>
       </c>
-      <c r="P32" s="2">
+      <c r="P32" s="1">
         <v>3</v>
       </c>
       <c r="Q32">
@@ -3216,7 +3221,7 @@
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A33" s="3">
+      <c r="A33" s="2">
         <v>20201203</v>
       </c>
       <c r="B33" t="s">
@@ -3225,38 +3230,38 @@
       <c r="C33" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
         <v>5</v>
       </c>
-      <c r="F33" s="2">
-        <v>0</v>
-      </c>
-      <c r="G33" s="2">
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
         <v>31</v>
       </c>
-      <c r="H33" s="2">
-        <v>0</v>
-      </c>
-      <c r="I33" s="2">
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
         <v>13</v>
       </c>
-      <c r="J33" s="2">
-        <v>0</v>
-      </c>
-      <c r="K33" s="2">
-        <v>0</v>
-      </c>
-      <c r="L33" s="2">
-        <v>0</v>
-      </c>
-      <c r="M33" s="2">
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
         <f t="shared" si="3"/>
         <v>82.81</v>
       </c>
-      <c r="N33" s="2">
+      <c r="N33" s="1">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
@@ -3285,7 +3290,7 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
+      <c r="A34" s="2">
         <v>20201203</v>
       </c>
       <c r="B34" t="s">
@@ -3294,38 +3299,38 @@
       <c r="C34" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="2">
-        <v>0</v>
-      </c>
-      <c r="E34" s="2">
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
         <v>8</v>
       </c>
-      <c r="F34" s="2">
-        <v>0</v>
-      </c>
-      <c r="G34" s="2">
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
         <v>2</v>
       </c>
-      <c r="H34" s="2">
-        <v>0</v>
-      </c>
-      <c r="I34" s="2">
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
         <v>22</v>
       </c>
-      <c r="J34" s="2">
-        <v>0</v>
-      </c>
-      <c r="K34" s="2">
-        <v>0</v>
-      </c>
-      <c r="L34" s="2">
-        <v>0</v>
-      </c>
-      <c r="M34" s="2">
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
         <f t="shared" si="3"/>
         <v>54.080000000000005</v>
       </c>
-      <c r="N34" s="2">
+      <c r="N34" s="1">
         <v>30</v>
       </c>
       <c r="O34">
@@ -3360,6 +3365,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8280A668-E5DD-416E-9A0F-EAD560AD754B}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3378,49 +3384,49 @@
       <c r="C1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="13">
+      <c r="D1" s="11">
         <v>44181.393055555556</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3428,25 +3434,25 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="8">
         <v>532.44000000000005</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="8">
         <v>788.58900000000006</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="8">
         <v>879.09799999999996</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="9" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3454,25 +3460,25 @@
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <v>345.863</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>543.33199999999999</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <v>615.14800000000002</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="9" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3480,25 +3486,25 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="8">
         <v>193.77600000000001</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>215.35300000000001</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="8">
         <v>222.47399999999999</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3506,25 +3512,25 @@
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="8">
         <v>558.18100000000004</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="8">
         <v>624.125</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="8">
         <v>645.89300000000003</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3532,25 +3538,25 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>393.15499999999997</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="8">
         <v>469.77699999999999</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="8">
         <v>494.72899999999998</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="9" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3558,25 +3564,25 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <v>231.80600000000001</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="8">
         <v>261.63799999999998</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="8">
         <v>271.423</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="9" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3584,25 +3590,25 @@
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="8">
         <v>360.48599999999999</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="8">
         <v>396.48700000000002</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="8">
         <v>408.48700000000002</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3610,25 +3616,25 @@
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="8">
         <v>155.262</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="8">
         <v>170.54300000000001</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="8">
         <v>175.57300000000001</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="9" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3636,46 +3642,46 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="8">
         <v>376.03</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="8">
         <v>420.91300000000001</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="8">
         <v>435.75299999999999</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="9" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>